<commit_message>
Fixed the data preprocessing - will now contain data for 34 states Updated jsonStateNamesIds.xlsx with separate column for datasets as some names didn't match the data Started work on a date slider Reworked .css to dynamically float divs based on content width (should lead to two-rowed layout)
</commit_message>
<xml_diff>
--- a/scripts/data/jsonStateNamesIDs.xlsx
+++ b/scripts/data/jsonStateNamesIDs.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\_Projects\TU Wien - Data Science\SS 2021\InfVis\Pr3\infvis-tuwien-sdg-covid\scripts\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94640C6F-44F4-4937-BD4E-3B5C3398A0E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - State Names" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - State Names" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>State Names</t>
   </si>
@@ -22,9 +31,6 @@
     <t>ID name</t>
   </si>
   <si>
-    <t>Andaman and Nicobar</t>
-  </si>
-  <si>
     <t xml:space="preserve">AN
 </t>
   </si>
@@ -299,15 +305,128 @@
   <si>
     <t xml:space="preserve">WB
 </t>
+  </si>
+  <si>
+    <t>Andaman and Nicobar Islands</t>
+  </si>
+  <si>
+    <t>Dataset name</t>
+  </si>
+  <si>
+    <t>Andhra Pradesh</t>
+  </si>
+  <si>
+    <t>Arunachal Pradesh</t>
+  </si>
+  <si>
+    <t>Assam</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>Chhattisgarh</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+  <si>
+    <t>Gujarat</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>Himachal Pradesh</t>
+  </si>
+  <si>
+    <t>Jammu and Kashmir</t>
+  </si>
+  <si>
+    <t>Jharkhand</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Lakshadweep</t>
+  </si>
+  <si>
+    <t>Madhya Pradesh</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Manipur</t>
+  </si>
+  <si>
+    <t>Meghalaya</t>
+  </si>
+  <si>
+    <t>Mizoram</t>
+  </si>
+  <si>
+    <t>Nagaland</t>
+  </si>
+  <si>
+    <t>Odisha</t>
+  </si>
+  <si>
+    <t>Puducherry</t>
+  </si>
+  <si>
+    <t>Punjab</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Sikkim</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Tripura</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>Uttarakhand</t>
+  </si>
+  <si>
+    <t>West Bengal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Telangana
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE
+</t>
+  </si>
+  <si>
+    <t>Telangana</t>
+  </si>
+  <si>
+    <t>NOT CONSIDERED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -430,63 +549,122 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -685,7 +863,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -704,7 +882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -734,7 +912,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,7 +938,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -786,7 +964,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +990,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,7 +1016,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -864,7 +1042,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -890,7 +1068,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -916,7 +1094,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -942,7 +1120,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -955,9 +1133,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -974,7 +1158,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -993,7 +1177,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +1203,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1229,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1071,7 +1255,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,7 +1281,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1123,7 +1307,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1333,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1359,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1385,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1411,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1240,9 +1424,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1256,7 +1446,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1275,7 +1465,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1495,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1521,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1547,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1573,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1409,7 +1599,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1435,7 +1625,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1461,7 +1651,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1487,7 +1677,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1513,7 +1703,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1526,330 +1716,459 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:B37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:3" ht="27.6" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" ht="20.2" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" ht="20.25" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" ht="32.2" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="C3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" ht="32" customHeight="1">
-      <c r="A4" t="s" s="6">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="7">
+      <c r="C4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" ht="44" customHeight="1">
-      <c r="A5" t="s" s="6">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s" s="7">
+      <c r="C5" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" ht="32" customHeight="1">
-      <c r="A6" t="s" s="6">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s" s="7">
+      <c r="C6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" ht="32" customHeight="1">
-      <c r="A7" t="s" s="6">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s" s="7">
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" ht="32" customHeight="1">
-      <c r="A8" t="s" s="6">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s" s="7">
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" ht="32" customHeight="1">
-      <c r="A9" t="s" s="6">
+      <c r="B9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s" s="7">
+      <c r="C9" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" ht="44" customHeight="1">
-      <c r="A10" t="s" s="6">
+      <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s" s="7">
+      <c r="C10" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" ht="32" customHeight="1">
-      <c r="A11" t="s" s="6">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s" s="7">
+      <c r="C11" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" ht="32" customHeight="1">
-      <c r="A12" t="s" s="6">
+      <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s" s="7">
+      <c r="C12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" ht="32" customHeight="1">
-      <c r="A13" t="s" s="6">
+      <c r="B13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s" s="7">
+      <c r="C13" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" ht="32" customHeight="1">
-      <c r="A14" t="s" s="6">
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B14" t="s" s="7">
+      <c r="C14" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" ht="32" customHeight="1">
-      <c r="A15" t="s" s="6">
+      <c r="B15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s" s="7">
+      <c r="C15" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" ht="44" customHeight="1">
-      <c r="A16" t="s" s="6">
+      <c r="B16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s" s="7">
+      <c r="C16" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" ht="44" customHeight="1">
-      <c r="A17" t="s" s="6">
+      <c r="B17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s" s="7">
+      <c r="C17" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A18" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" ht="32" customHeight="1">
-      <c r="A18" t="s" s="6">
+      <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s" s="7">
+      <c r="C18" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" ht="32" customHeight="1">
-      <c r="A19" t="s" s="6">
+      <c r="B19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s" s="7">
+      <c r="C19" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" ht="32" customHeight="1">
-      <c r="A20" t="s" s="6">
+      <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B20" t="s" s="7">
+      <c r="C20" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" ht="32" customHeight="1">
-      <c r="A21" t="s" s="6">
+      <c r="B21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B21" t="s" s="7">
+      <c r="C21" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A22" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" ht="32" customHeight="1">
-      <c r="A22" t="s" s="6">
+      <c r="B22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s" s="7">
+      <c r="C22" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" ht="32" customHeight="1">
-      <c r="A23" t="s" s="6">
+      <c r="B23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B23" t="s" s="7">
+      <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A24" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" ht="32" customHeight="1">
-      <c r="A24" t="s" s="6">
+      <c r="B24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s" s="7">
+      <c r="C24" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A25" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" ht="32" customHeight="1">
-      <c r="A25" t="s" s="6">
+      <c r="B25" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s" s="7">
+      <c r="C25" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" ht="32" customHeight="1">
-      <c r="A26" t="s" s="6">
+      <c r="B26" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s" s="7">
+      <c r="C26" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" ht="32" customHeight="1">
-      <c r="A27" t="s" s="6">
+      <c r="B27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s" s="7">
+      <c r="C27" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" ht="32" customHeight="1">
-      <c r="A28" t="s" s="6">
+      <c r="B28" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s" s="7">
+      <c r="C28" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A29" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" ht="32" customHeight="1">
-      <c r="A29" t="s" s="6">
+      <c r="B29" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B29" t="s" s="7">
+      <c r="C29" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A30" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" ht="32" customHeight="1">
-      <c r="A30" t="s" s="6">
+      <c r="B30" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B30" t="s" s="7">
+      <c r="C30" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A31" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" ht="32" customHeight="1">
-      <c r="A31" t="s" s="6">
+      <c r="B31" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B31" t="s" s="7">
+      <c r="C31" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A32" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" ht="32" customHeight="1">
-      <c r="A32" t="s" s="6">
+      <c r="B32" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s" s="7">
+      <c r="C32" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A33" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" ht="32" customHeight="1">
-      <c r="A33" t="s" s="6">
+      <c r="B33" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B33" t="s" s="7">
+      <c r="C33" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A35" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" ht="32" customHeight="1">
-      <c r="A34" t="s" s="6">
+      <c r="B35" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B34" t="s" s="7">
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A36" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" ht="32" customHeight="1">
-      <c r="A35" t="s" s="6">
+      <c r="B36" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B35" t="s" s="7">
+      <c r="C36" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A37" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" ht="32" customHeight="1">
-      <c r="A36" t="s" s="6">
+      <c r="B37" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B36" t="s" s="7">
+      <c r="C37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A38" s="5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" ht="32" customHeight="1">
-      <c r="A37" t="s" s="6">
+      <c r="B38" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B37" t="s" s="7">
-        <v>72</v>
+      <c r="C38" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>